<commit_message>
fixed area calculation bug
Processing times increased again, but the area was being multiplied by the number of habitat metrics
</commit_message>
<xml_diff>
--- a/Cherry_Braid_AQ.xlsx
+++ b/Cherry_Braid_AQ.xlsx
@@ -9,10 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Cherry_Braid_AQ" sheetId="2" r:id="rId1"/>
+    <sheet name="10day" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="23">
   <si>
     <t>discharge</t>
   </si>
@@ -53,9 +54,6 @@
     <t>speckleddace</t>
   </si>
   <si>
-    <t>Calculated</t>
-  </si>
-  <si>
     <t>Reported</t>
   </si>
   <si>
@@ -64,13 +62,46 @@
   <si>
     <t>sonoransucker</t>
   </si>
+  <si>
+    <t>Calculated slow speed</t>
+  </si>
+  <si>
+    <t>Calculated fast speed</t>
+  </si>
+  <si>
+    <t>% Error</t>
+  </si>
+  <si>
+    <t>year</t>
+  </si>
+  <si>
+    <t>month</t>
+  </si>
+  <si>
+    <t>MonAvgLowArea</t>
+  </si>
+  <si>
+    <t>Reported Min 10-day mean</t>
+  </si>
+  <si>
+    <t>EP edits Reported 10-day mean</t>
+  </si>
+  <si>
+    <t>Speckled Dace</t>
+  </si>
+  <si>
+    <t>Longfin Dace</t>
+  </si>
+  <si>
+    <t>EP edits</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
-    <numFmt numFmtId="168" formatCode="#,##0.0"/>
+    <numFmt numFmtId="164" formatCode="#,##0.0"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -87,7 +118,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -106,8 +137,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="4">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -150,24 +187,148 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF999999"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color rgb="FF999999"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color rgb="FF999999"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF999999"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF999999"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -448,10 +609,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T44"/>
+  <dimension ref="A1:T67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="U23" sqref="U23"/>
+    <sheetView topLeftCell="F40" workbookViewId="0">
+      <selection activeCell="O71" sqref="O71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -472,10 +633,10 @@
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>9</v>
+      </c>
+      <c r="L1" t="s">
         <v>10</v>
-      </c>
-      <c r="L1" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.25">
@@ -492,7 +653,7 @@
         <v>1</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>4</v>
@@ -519,7 +680,7 @@
         <v>1</v>
       </c>
       <c r="O2" s="7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="P2" s="1" t="s">
         <v>4</v>
@@ -1899,7 +2060,7 @@
     </row>
     <row r="23" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A23" s="6" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="B23" s="6"/>
       <c r="C23" s="6"/>
@@ -1925,7 +2086,7 @@
         <v>1</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F24" s="1" t="s">
         <v>4</v>
@@ -2207,7 +2368,7 @@
       </c>
       <c r="K32" s="8"/>
     </row>
-    <row r="33" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="5">
         <v>125</v>
       </c>
@@ -2240,7 +2401,7 @@
       </c>
       <c r="K33" s="8"/>
     </row>
-    <row r="34" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="5">
         <v>200</v>
       </c>
@@ -2273,7 +2434,7 @@
       </c>
       <c r="K34" s="8"/>
     </row>
-    <row r="35" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="5">
         <v>250</v>
       </c>
@@ -2306,7 +2467,7 @@
       </c>
       <c r="K35" s="8"/>
     </row>
-    <row r="36" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="5">
         <v>400</v>
       </c>
@@ -2339,7 +2500,7 @@
       </c>
       <c r="K36" s="8"/>
     </row>
-    <row r="37" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="5">
         <v>500</v>
       </c>
@@ -2372,7 +2533,7 @@
       </c>
       <c r="K37" s="8"/>
     </row>
-    <row r="38" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="5">
         <v>750</v>
       </c>
@@ -2405,7 +2566,7 @@
       </c>
       <c r="K38" s="8"/>
     </row>
-    <row r="39" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="5">
         <v>1000</v>
       </c>
@@ -2438,7 +2599,7 @@
       </c>
       <c r="K39" s="8"/>
     </row>
-    <row r="40" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" s="5">
         <v>2000</v>
       </c>
@@ -2471,7 +2632,7 @@
       </c>
       <c r="K40" s="8"/>
     </row>
-    <row r="41" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41" s="5">
         <v>2500</v>
       </c>
@@ -2504,7 +2665,7 @@
       </c>
       <c r="K41" s="8"/>
     </row>
-    <row r="42" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" s="5">
         <v>3800</v>
       </c>
@@ -2537,7 +2698,7 @@
       </c>
       <c r="K42" s="8"/>
     </row>
-    <row r="43" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" s="5">
         <v>5000</v>
       </c>
@@ -2570,7 +2731,7 @@
       </c>
       <c r="K43" s="8"/>
     </row>
-    <row r="44" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A44" s="5">
         <v>10000</v>
       </c>
@@ -2602,6 +2763,2128 @@
         <v>1463.32</v>
       </c>
       <c r="K44" s="8"/>
+    </row>
+    <row r="45" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="46" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A46" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="B46" s="11"/>
+      <c r="C46" s="11"/>
+      <c r="D46" s="11"/>
+      <c r="E46" s="11"/>
+      <c r="F46" s="11"/>
+      <c r="G46" s="11"/>
+      <c r="H46" s="11"/>
+      <c r="I46" s="11"/>
+      <c r="J46" s="11"/>
+      <c r="L46" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="M46" s="13"/>
+      <c r="N46" s="13"/>
+      <c r="O46" s="13"/>
+      <c r="P46" s="13"/>
+      <c r="Q46" s="13"/>
+      <c r="R46" s="13"/>
+      <c r="S46" s="13"/>
+      <c r="T46" s="14"/>
+    </row>
+    <row r="47" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A47" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="B47" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="C47" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="D47" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="E47" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="F47" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="G47" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="H47" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="I47" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="J47" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="L47" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="M47" s="16" t="s">
+        <v>3</v>
+      </c>
+      <c r="N47" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="O47" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="P47" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q47" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="R47" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="S47" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="T47" s="17" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="48" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A48" s="11">
+        <v>4.8</v>
+      </c>
+      <c r="B48" s="11">
+        <v>7063.0119999999997</v>
+      </c>
+      <c r="C48" s="11">
+        <v>6917.1109999999999</v>
+      </c>
+      <c r="D48" s="11">
+        <v>5416.393</v>
+      </c>
+      <c r="E48" s="11">
+        <v>4350.2049999999999</v>
+      </c>
+      <c r="F48" s="11">
+        <v>4375.82</v>
+      </c>
+      <c r="G48" s="11">
+        <v>1921.6189999999999</v>
+      </c>
+      <c r="H48" s="11">
+        <v>4351.0249999999996</v>
+      </c>
+      <c r="I48" s="11">
+        <v>4573.9750000000004</v>
+      </c>
+      <c r="J48" s="11">
+        <v>2094.3649999999998</v>
+      </c>
+      <c r="L48" s="15">
+        <f>(B48-B3)/B3*100</f>
+        <v>-0.24788759401798638</v>
+      </c>
+      <c r="M48" s="16">
+        <f t="shared" ref="M48:T48" si="10">(C48-C3)/C3*100</f>
+        <v>0.23041953684198291</v>
+      </c>
+      <c r="N48" s="16">
+        <f t="shared" si="10"/>
+        <v>-0.94118964445169506</v>
+      </c>
+      <c r="O48" s="16">
+        <f t="shared" si="10"/>
+        <v>-0.40399273711462286</v>
+      </c>
+      <c r="P48" s="16">
+        <f t="shared" si="10"/>
+        <v>0.15842354128539338</v>
+      </c>
+      <c r="Q48" s="16">
+        <f t="shared" si="10"/>
+        <v>-0.32714945209010354</v>
+      </c>
+      <c r="R48" s="16">
+        <f t="shared" si="10"/>
+        <v>0.21331095731329913</v>
+      </c>
+      <c r="S48" s="16">
+        <f t="shared" si="10"/>
+        <v>-0.16575647186948159</v>
+      </c>
+      <c r="T48" s="17">
+        <f t="shared" si="10"/>
+        <v>-1.9012179625454328</v>
+      </c>
+    </row>
+    <row r="49" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A49" s="11">
+        <v>10</v>
+      </c>
+      <c r="B49" s="11">
+        <v>8181.3519999999999</v>
+      </c>
+      <c r="C49" s="11">
+        <v>8030.02</v>
+      </c>
+      <c r="D49" s="11">
+        <v>6083.607</v>
+      </c>
+      <c r="E49" s="11">
+        <v>5979.201</v>
+      </c>
+      <c r="F49" s="11">
+        <v>4818.34</v>
+      </c>
+      <c r="G49" s="11">
+        <v>2321.3110000000001</v>
+      </c>
+      <c r="H49" s="11">
+        <v>4757.1719999999996</v>
+      </c>
+      <c r="I49" s="11">
+        <v>4925.5119999999997</v>
+      </c>
+      <c r="J49" s="11">
+        <v>3033.5039999999999</v>
+      </c>
+      <c r="L49" s="15">
+        <f t="shared" ref="L49:L67" si="11">(B49-B4)/B4*100</f>
+        <v>-0.20443727443608262</v>
+      </c>
+      <c r="M49" s="16">
+        <f t="shared" ref="M49:M67" si="12">(C49-C4)/C4*100</f>
+        <v>0.18663474072801312</v>
+      </c>
+      <c r="N49" s="16">
+        <f t="shared" ref="N49:N67" si="13">(D49-D4)/D4*100</f>
+        <v>-0.84262411536451509</v>
+      </c>
+      <c r="O49" s="16">
+        <f t="shared" ref="O49:O67" si="14">(E49-E4)/E4*100</f>
+        <v>-0.65502505383742438</v>
+      </c>
+      <c r="P49" s="16">
+        <f t="shared" ref="P49:P67" si="15">(F49-F4)/F4*100</f>
+        <v>5.1990562254715107E-2</v>
+      </c>
+      <c r="Q49" s="16">
+        <f t="shared" ref="Q49:Q67" si="16">(G49-G4)/G4*100</f>
+        <v>-9.8488658866308934E-2</v>
+      </c>
+      <c r="R49" s="16">
+        <f t="shared" ref="R49:R67" si="17">(H49-H4)/H4*100</f>
+        <v>0.3308834922599867</v>
+      </c>
+      <c r="S49" s="16">
+        <f t="shared" ref="S49:S67" si="18">(I49-I4)/I4*100</f>
+        <v>-0.3572360261574502</v>
+      </c>
+      <c r="T49" s="17">
+        <f t="shared" ref="T49:T67" si="19">(J49-J4)/J4*100</f>
+        <v>-1.4436262994070002</v>
+      </c>
+    </row>
+    <row r="50" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A50" s="11">
+        <v>20</v>
+      </c>
+      <c r="B50" s="11">
+        <v>8506.3520000000008</v>
+      </c>
+      <c r="C50" s="11">
+        <v>8670.7990000000009</v>
+      </c>
+      <c r="D50" s="11">
+        <v>6373.6679999999997</v>
+      </c>
+      <c r="E50" s="11">
+        <v>7117.52</v>
+      </c>
+      <c r="F50" s="11">
+        <v>5176.5370000000003</v>
+      </c>
+      <c r="G50" s="11">
+        <v>2597.1309999999999</v>
+      </c>
+      <c r="H50" s="11">
+        <v>4928.9960000000001</v>
+      </c>
+      <c r="I50" s="11">
+        <v>5117.6229999999996</v>
+      </c>
+      <c r="J50" s="11">
+        <v>3541.598</v>
+      </c>
+      <c r="L50" s="15">
+        <f t="shared" si="11"/>
+        <v>-0.3339157579098706</v>
+      </c>
+      <c r="M50" s="16">
+        <f t="shared" si="12"/>
+        <v>0.11796311851967281</v>
+      </c>
+      <c r="N50" s="16">
+        <f t="shared" si="13"/>
+        <v>-0.87804423013683031</v>
+      </c>
+      <c r="O50" s="16">
+        <f t="shared" si="14"/>
+        <v>-0.69552794704736942</v>
+      </c>
+      <c r="P50" s="16">
+        <f t="shared" si="15"/>
+        <v>-8.5158365111068196E-2</v>
+      </c>
+      <c r="Q50" s="16">
+        <f t="shared" si="16"/>
+        <v>-0.2366719397709604</v>
+      </c>
+      <c r="R50" s="16">
+        <f t="shared" si="17"/>
+        <v>0.36212870051233004</v>
+      </c>
+      <c r="S50" s="16">
+        <f t="shared" si="18"/>
+        <v>-0.12662913137867149</v>
+      </c>
+      <c r="T50" s="17">
+        <f t="shared" si="19"/>
+        <v>-0.60439664312593244</v>
+      </c>
+    </row>
+    <row r="51" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A51" s="11">
+        <v>25</v>
+      </c>
+      <c r="B51" s="11">
+        <v>8465.8809999999994</v>
+      </c>
+      <c r="C51" s="11">
+        <v>8697.9509999999991</v>
+      </c>
+      <c r="D51" s="11">
+        <v>6275.3069999999998</v>
+      </c>
+      <c r="E51" s="11">
+        <v>7326.6390000000001</v>
+      </c>
+      <c r="F51" s="11">
+        <v>5130.43</v>
+      </c>
+      <c r="G51" s="11">
+        <v>2718.34</v>
+      </c>
+      <c r="H51" s="11">
+        <v>4418.2380000000003</v>
+      </c>
+      <c r="I51" s="11">
+        <v>4582.2749999999996</v>
+      </c>
+      <c r="J51" s="11">
+        <v>3696.721</v>
+      </c>
+      <c r="L51" s="15">
+        <f t="shared" si="11"/>
+        <v>-0.20909432176197357</v>
+      </c>
+      <c r="M51" s="16">
+        <f t="shared" si="12"/>
+        <v>0.14035460044313294</v>
+      </c>
+      <c r="N51" s="16">
+        <f t="shared" si="13"/>
+        <v>-0.84771862655690144</v>
+      </c>
+      <c r="O51" s="16">
+        <f t="shared" si="14"/>
+        <v>-0.73914554049262149</v>
+      </c>
+      <c r="P51" s="16">
+        <f t="shared" si="15"/>
+        <v>-6.9279715862488822E-2</v>
+      </c>
+      <c r="Q51" s="16">
+        <f t="shared" si="16"/>
+        <v>0.13470696336340171</v>
+      </c>
+      <c r="R51" s="16">
+        <f t="shared" si="17"/>
+        <v>0.46553128694715157</v>
+      </c>
+      <c r="S51" s="16">
+        <f t="shared" si="18"/>
+        <v>-0.12909546485685822</v>
+      </c>
+      <c r="T51" s="17">
+        <f t="shared" si="19"/>
+        <v>-0.68521066550291998</v>
+      </c>
+    </row>
+    <row r="52" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A52" s="11">
+        <v>33</v>
+      </c>
+      <c r="B52" s="11">
+        <v>8408.607</v>
+      </c>
+      <c r="C52" s="11">
+        <v>8738.73</v>
+      </c>
+      <c r="D52" s="11">
+        <v>6172.7460000000001</v>
+      </c>
+      <c r="E52" s="11">
+        <v>7553.1760000000004</v>
+      </c>
+      <c r="F52" s="11">
+        <v>5136.3729999999996</v>
+      </c>
+      <c r="G52" s="11">
+        <v>2733.5039999999999</v>
+      </c>
+      <c r="H52" s="11">
+        <v>3194.2620000000002</v>
+      </c>
+      <c r="I52" s="11">
+        <v>3426.23</v>
+      </c>
+      <c r="J52" s="11">
+        <v>3820.799</v>
+      </c>
+      <c r="L52" s="15">
+        <f t="shared" si="11"/>
+        <v>-0.32514653524594334</v>
+      </c>
+      <c r="M52" s="16">
+        <f t="shared" si="12"/>
+        <v>0.26570833955244344</v>
+      </c>
+      <c r="N52" s="16">
+        <f t="shared" si="13"/>
+        <v>-0.86892819483187345</v>
+      </c>
+      <c r="O52" s="16">
+        <f t="shared" si="14"/>
+        <v>-0.50891641107524144</v>
+      </c>
+      <c r="P52" s="16">
+        <f t="shared" si="15"/>
+        <v>-0.26724956610562794</v>
+      </c>
+      <c r="Q52" s="16">
+        <f t="shared" si="16"/>
+        <v>0.31783525022397779</v>
+      </c>
+      <c r="R52" s="16">
+        <f t="shared" si="17"/>
+        <v>0.79672360429167421</v>
+      </c>
+      <c r="S52" s="16">
+        <f t="shared" si="18"/>
+        <v>-8.0733273870059991E-2</v>
+      </c>
+      <c r="T52" s="17">
+        <f t="shared" si="19"/>
+        <v>-0.56422566433479315</v>
+      </c>
+    </row>
+    <row r="53" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A53" s="11">
+        <v>59</v>
+      </c>
+      <c r="B53" s="11">
+        <v>6925.3069999999998</v>
+      </c>
+      <c r="C53" s="11">
+        <v>6772.951</v>
+      </c>
+      <c r="D53" s="11">
+        <v>5801.5370000000003</v>
+      </c>
+      <c r="E53" s="11">
+        <v>7326.8440000000001</v>
+      </c>
+      <c r="F53" s="11">
+        <v>4949.7950000000001</v>
+      </c>
+      <c r="G53" s="11">
+        <v>2710.0410000000002</v>
+      </c>
+      <c r="H53" s="11">
+        <v>2058.5039999999999</v>
+      </c>
+      <c r="I53" s="11">
+        <v>2226.7420000000002</v>
+      </c>
+      <c r="J53" s="11">
+        <v>3927.4589999999998</v>
+      </c>
+      <c r="L53" s="15">
+        <f t="shared" si="11"/>
+        <v>-0.45098646796218445</v>
+      </c>
+      <c r="M53" s="16">
+        <f t="shared" si="12"/>
+        <v>0.30826139724484675</v>
+      </c>
+      <c r="N53" s="16">
+        <f t="shared" si="13"/>
+        <v>-0.6074395162696431</v>
+      </c>
+      <c r="O53" s="16">
+        <f t="shared" si="14"/>
+        <v>-0.52573012902032878</v>
+      </c>
+      <c r="P53" s="16">
+        <f t="shared" si="15"/>
+        <v>-7.1954085268073231E-2</v>
+      </c>
+      <c r="Q53" s="16">
+        <f t="shared" si="16"/>
+        <v>0.5541787179892036</v>
+      </c>
+      <c r="R53" s="16">
+        <f t="shared" si="17"/>
+        <v>0.62135361088400654</v>
+      </c>
+      <c r="S53" s="16">
+        <f t="shared" si="18"/>
+        <v>0.24264235656520933</v>
+      </c>
+      <c r="T53" s="17">
+        <f t="shared" si="19"/>
+        <v>-0.67715585416361856</v>
+      </c>
+    </row>
+    <row r="54" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A54" s="11">
+        <v>80</v>
+      </c>
+      <c r="B54" s="11">
+        <v>5924.4880000000003</v>
+      </c>
+      <c r="C54" s="11">
+        <v>5578.1760000000004</v>
+      </c>
+      <c r="D54" s="11">
+        <v>4919.6719999999996</v>
+      </c>
+      <c r="E54" s="11">
+        <v>7106.1480000000001</v>
+      </c>
+      <c r="F54" s="11">
+        <v>4179.6109999999999</v>
+      </c>
+      <c r="G54" s="11">
+        <v>2383.0940000000001</v>
+      </c>
+      <c r="H54" s="11">
+        <v>1570.0820000000001</v>
+      </c>
+      <c r="I54" s="11">
+        <v>1713.627</v>
+      </c>
+      <c r="J54" s="11">
+        <v>3859.3240000000001</v>
+      </c>
+      <c r="L54" s="15">
+        <f t="shared" si="11"/>
+        <v>-0.5351586153614184</v>
+      </c>
+      <c r="M54" s="16">
+        <f t="shared" si="12"/>
+        <v>6.0047720060058173E-2</v>
+      </c>
+      <c r="N54" s="16">
+        <f t="shared" si="13"/>
+        <v>-1.0182077809827359</v>
+      </c>
+      <c r="O54" s="16">
+        <f t="shared" si="14"/>
+        <v>-0.56378694732645196</v>
+      </c>
+      <c r="P54" s="16">
+        <f t="shared" si="15"/>
+        <v>-0.43318983224850455</v>
+      </c>
+      <c r="Q54" s="16">
+        <f t="shared" si="16"/>
+        <v>0.17973076955961845</v>
+      </c>
+      <c r="R54" s="16">
+        <f t="shared" si="17"/>
+        <v>1.6776886216604978</v>
+      </c>
+      <c r="S54" s="16">
+        <f t="shared" si="18"/>
+        <v>0.63364252517169417</v>
+      </c>
+      <c r="T54" s="17">
+        <f t="shared" si="19"/>
+        <v>-0.78205401577918243</v>
+      </c>
+    </row>
+    <row r="55" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A55" s="11">
+        <v>100</v>
+      </c>
+      <c r="B55" s="11">
+        <v>6437.2950000000001</v>
+      </c>
+      <c r="C55" s="11">
+        <v>6080.2250000000004</v>
+      </c>
+      <c r="D55" s="11">
+        <v>5148.3609999999999</v>
+      </c>
+      <c r="E55" s="11">
+        <v>7493.34</v>
+      </c>
+      <c r="F55" s="11">
+        <v>4389.3440000000001</v>
+      </c>
+      <c r="G55" s="11">
+        <v>2474.7950000000001</v>
+      </c>
+      <c r="H55" s="11">
+        <v>2048.2579999999998</v>
+      </c>
+      <c r="I55" s="11">
+        <v>2324.1799999999998</v>
+      </c>
+      <c r="J55" s="11">
+        <v>4246.2089999999998</v>
+      </c>
+      <c r="L55" s="15">
+        <f t="shared" si="11"/>
+        <v>-0.15688467715299934</v>
+      </c>
+      <c r="M55" s="16">
+        <f t="shared" si="12"/>
+        <v>0.22580507388682999</v>
+      </c>
+      <c r="N55" s="16">
+        <f t="shared" si="13"/>
+        <v>-0.74826473941076377</v>
+      </c>
+      <c r="O55" s="16">
+        <f t="shared" si="14"/>
+        <v>-0.63665426057181185</v>
+      </c>
+      <c r="P55" s="16">
+        <f t="shared" si="15"/>
+        <v>7.4830561902000492E-2</v>
+      </c>
+      <c r="Q55" s="16">
+        <f t="shared" si="16"/>
+        <v>-0.47035800043838183</v>
+      </c>
+      <c r="R55" s="16">
+        <f t="shared" si="17"/>
+        <v>1.4389765701599384</v>
+      </c>
+      <c r="S55" s="16">
+        <f t="shared" si="18"/>
+        <v>0.45740290273558482</v>
+      </c>
+      <c r="T55" s="17">
+        <f t="shared" si="19"/>
+        <v>-0.51087310365612615</v>
+      </c>
+    </row>
+    <row r="56" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A56" s="11">
+        <v>125</v>
+      </c>
+      <c r="B56" s="11">
+        <v>6213.6270000000004</v>
+      </c>
+      <c r="C56" s="11">
+        <v>5841.8029999999999</v>
+      </c>
+      <c r="D56" s="11">
+        <v>4917.3159999999998</v>
+      </c>
+      <c r="E56" s="11">
+        <v>7101.4340000000002</v>
+      </c>
+      <c r="F56" s="11">
+        <v>4096.2089999999998</v>
+      </c>
+      <c r="G56" s="11">
+        <v>2302.7660000000001</v>
+      </c>
+      <c r="H56" s="11">
+        <v>1878.279</v>
+      </c>
+      <c r="I56" s="11">
+        <v>2107.377</v>
+      </c>
+      <c r="J56" s="11">
+        <v>4444.0569999999998</v>
+      </c>
+      <c r="L56" s="15">
+        <f t="shared" si="11"/>
+        <v>-0.33662225166701254</v>
+      </c>
+      <c r="M56" s="16">
+        <f t="shared" si="12"/>
+        <v>0.19001853978501854</v>
+      </c>
+      <c r="N56" s="16">
+        <f t="shared" si="13"/>
+        <v>-0.75524564560697283</v>
+      </c>
+      <c r="O56" s="16">
+        <f t="shared" si="14"/>
+        <v>-0.56854568703768704</v>
+      </c>
+      <c r="P56" s="16">
+        <f t="shared" si="15"/>
+        <v>0.11519094298640595</v>
+      </c>
+      <c r="Q56" s="16">
+        <f t="shared" si="16"/>
+        <v>-0.54488642353839234</v>
+      </c>
+      <c r="R56" s="16">
+        <f t="shared" si="17"/>
+        <v>1.0696434784906377</v>
+      </c>
+      <c r="S56" s="16">
+        <f t="shared" si="18"/>
+        <v>0.37299621314970005</v>
+      </c>
+      <c r="T56" s="17">
+        <f t="shared" si="19"/>
+        <v>-0.39474862867816152</v>
+      </c>
+    </row>
+    <row r="57" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A57" s="11">
+        <v>200</v>
+      </c>
+      <c r="B57" s="11">
+        <v>5024.3850000000002</v>
+      </c>
+      <c r="C57" s="11">
+        <v>4692.3159999999998</v>
+      </c>
+      <c r="D57" s="11">
+        <v>3827.971</v>
+      </c>
+      <c r="E57" s="11">
+        <v>5702.4589999999998</v>
+      </c>
+      <c r="F57" s="11">
+        <v>3253.0740000000001</v>
+      </c>
+      <c r="G57" s="11">
+        <v>1633.7090000000001</v>
+      </c>
+      <c r="H57" s="11">
+        <v>1590.3689999999999</v>
+      </c>
+      <c r="I57" s="11">
+        <v>1802.7660000000001</v>
+      </c>
+      <c r="J57" s="11">
+        <v>4073.9749999999999</v>
+      </c>
+      <c r="L57" s="15">
+        <f t="shared" si="11"/>
+        <v>-0.23632236275130328</v>
+      </c>
+      <c r="M57" s="16">
+        <f t="shared" si="12"/>
+        <v>0.56878730224829011</v>
+      </c>
+      <c r="N57" s="16">
+        <f t="shared" si="13"/>
+        <v>-1.3131567167646172</v>
+      </c>
+      <c r="O57" s="16">
+        <f t="shared" si="14"/>
+        <v>-0.73625088639768055</v>
+      </c>
+      <c r="P57" s="16">
+        <f t="shared" si="15"/>
+        <v>-0.38031205981069027</v>
+      </c>
+      <c r="Q57" s="16">
+        <f t="shared" si="16"/>
+        <v>-0.29943140534427626</v>
+      </c>
+      <c r="R57" s="16">
+        <f t="shared" si="17"/>
+        <v>1.6932414497179273</v>
+      </c>
+      <c r="S57" s="16">
+        <f t="shared" si="18"/>
+        <v>0.8532771241558591</v>
+      </c>
+      <c r="T57" s="17">
+        <f t="shared" si="19"/>
+        <v>-0.51962006741699751</v>
+      </c>
+    </row>
+    <row r="58" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A58" s="11">
+        <v>250</v>
+      </c>
+      <c r="B58" s="11">
+        <v>3750.2049999999999</v>
+      </c>
+      <c r="C58" s="11">
+        <v>3753.7910000000002</v>
+      </c>
+      <c r="D58" s="11">
+        <v>2741.2910000000002</v>
+      </c>
+      <c r="E58" s="11">
+        <v>3294.16</v>
+      </c>
+      <c r="F58" s="11">
+        <v>2431.4549999999999</v>
+      </c>
+      <c r="G58" s="11">
+        <v>1137.0899999999999</v>
+      </c>
+      <c r="H58" s="11">
+        <v>1333.0940000000001</v>
+      </c>
+      <c r="I58" s="11">
+        <v>1545.902</v>
+      </c>
+      <c r="J58" s="11">
+        <v>2486.8850000000002</v>
+      </c>
+      <c r="L58" s="15">
+        <f t="shared" si="11"/>
+        <v>-3.4996457333585709E-2</v>
+      </c>
+      <c r="M58" s="16">
+        <f t="shared" si="12"/>
+        <v>0.87165603685887916</v>
+      </c>
+      <c r="N58" s="16">
+        <f t="shared" si="13"/>
+        <v>-0.65320441585257005</v>
+      </c>
+      <c r="O58" s="16">
+        <f t="shared" si="14"/>
+        <v>-0.40651368446758768</v>
+      </c>
+      <c r="P58" s="16">
+        <f t="shared" si="15"/>
+        <v>6.98957520734097E-2</v>
+      </c>
+      <c r="Q58" s="16">
+        <f t="shared" si="16"/>
+        <v>0.83574919759293964</v>
+      </c>
+      <c r="R58" s="16">
+        <f t="shared" si="17"/>
+        <v>3.0015501518644232</v>
+      </c>
+      <c r="S58" s="16">
+        <f t="shared" si="18"/>
+        <v>1.6365455625043219</v>
+      </c>
+      <c r="T58" s="17">
+        <f t="shared" si="19"/>
+        <v>-0.40895461687868007</v>
+      </c>
+    </row>
+    <row r="59" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A59" s="11">
+        <v>400</v>
+      </c>
+      <c r="B59" s="11">
+        <v>3748.9749999999999</v>
+      </c>
+      <c r="C59" s="11">
+        <v>3794.57</v>
+      </c>
+      <c r="D59" s="11">
+        <v>2795.6970000000001</v>
+      </c>
+      <c r="E59" s="11">
+        <v>3015.8809999999999</v>
+      </c>
+      <c r="F59" s="11">
+        <v>2513.9340000000002</v>
+      </c>
+      <c r="G59" s="11">
+        <v>1125</v>
+      </c>
+      <c r="H59" s="11">
+        <v>1675.2049999999999</v>
+      </c>
+      <c r="I59" s="11">
+        <v>1702.2539999999999</v>
+      </c>
+      <c r="J59" s="11">
+        <v>2048.873</v>
+      </c>
+      <c r="L59" s="15">
+        <f t="shared" si="11"/>
+        <v>0.53090663889007195</v>
+      </c>
+      <c r="M59" s="16">
+        <f t="shared" si="12"/>
+        <v>1.0688126303196868</v>
+      </c>
+      <c r="N59" s="16">
+        <f t="shared" si="13"/>
+        <v>0.21864478371098106</v>
+      </c>
+      <c r="O59" s="16">
+        <f t="shared" si="14"/>
+        <v>0.22750508162438302</v>
+      </c>
+      <c r="P59" s="16">
+        <f t="shared" si="15"/>
+        <v>0.72248338249682165</v>
+      </c>
+      <c r="Q59" s="16">
+        <f t="shared" si="16"/>
+        <v>1.2859365823844398</v>
+      </c>
+      <c r="R59" s="16">
+        <f t="shared" si="17"/>
+        <v>1.1165916155405797</v>
+      </c>
+      <c r="S59" s="16">
+        <f t="shared" si="18"/>
+        <v>1.2797078930656716</v>
+      </c>
+      <c r="T59" s="17">
+        <f t="shared" si="19"/>
+        <v>0.33892918926757221</v>
+      </c>
+    </row>
+    <row r="60" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A60" s="11">
+        <v>500</v>
+      </c>
+      <c r="B60" s="11">
+        <v>5215.0609999999997</v>
+      </c>
+      <c r="C60" s="11">
+        <v>5326.8440000000001</v>
+      </c>
+      <c r="D60" s="11">
+        <v>4005.6350000000002</v>
+      </c>
+      <c r="E60" s="11">
+        <v>4155.6350000000002</v>
+      </c>
+      <c r="F60" s="11">
+        <v>3312.09</v>
+      </c>
+      <c r="G60" s="11">
+        <v>1915.5740000000001</v>
+      </c>
+      <c r="H60" s="11">
+        <v>2326.6390000000001</v>
+      </c>
+      <c r="I60" s="11">
+        <v>2323.0529999999999</v>
+      </c>
+      <c r="J60" s="11">
+        <v>2800.5120000000002</v>
+      </c>
+      <c r="L60" s="15">
+        <f t="shared" si="11"/>
+        <v>0.31853052684405558</v>
+      </c>
+      <c r="M60" s="16">
+        <f t="shared" si="12"/>
+        <v>0.8739572314908175</v>
+      </c>
+      <c r="N60" s="16">
+        <f t="shared" si="13"/>
+        <v>-0.10610540797736016</v>
+      </c>
+      <c r="O60" s="16">
+        <f t="shared" si="14"/>
+        <v>-0.22729107556421566</v>
+      </c>
+      <c r="P60" s="16">
+        <f t="shared" si="15"/>
+        <v>0.2875658575131041</v>
+      </c>
+      <c r="Q60" s="16">
+        <f t="shared" si="16"/>
+        <v>1.0239935137432714</v>
+      </c>
+      <c r="R60" s="16">
+        <f t="shared" si="17"/>
+        <v>1.1057247835140889</v>
+      </c>
+      <c r="S60" s="16">
+        <f t="shared" si="18"/>
+        <v>1.1736709126377971</v>
+      </c>
+      <c r="T60" s="17">
+        <f t="shared" si="19"/>
+        <v>-0.30759108497743465</v>
+      </c>
+    </row>
+    <row r="61" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A61" s="11">
+        <v>750</v>
+      </c>
+      <c r="B61" s="11">
+        <v>5871.107</v>
+      </c>
+      <c r="C61" s="11">
+        <v>5872.3360000000002</v>
+      </c>
+      <c r="D61" s="11">
+        <v>4827.2539999999999</v>
+      </c>
+      <c r="E61" s="11">
+        <v>5306.25</v>
+      </c>
+      <c r="F61" s="11">
+        <v>3796.6190000000001</v>
+      </c>
+      <c r="G61" s="11">
+        <v>2159.4259999999999</v>
+      </c>
+      <c r="H61" s="11">
+        <v>2430.123</v>
+      </c>
+      <c r="I61" s="11">
+        <v>2407.9920000000002</v>
+      </c>
+      <c r="J61" s="11">
+        <v>3474.8980000000001</v>
+      </c>
+      <c r="L61" s="15">
+        <f t="shared" si="11"/>
+        <v>0.75149263583550152</v>
+      </c>
+      <c r="M61" s="16">
+        <f t="shared" si="12"/>
+        <v>0.89155847189654414</v>
+      </c>
+      <c r="N61" s="16">
+        <f t="shared" si="13"/>
+        <v>0.82617568396003982</v>
+      </c>
+      <c r="O61" s="16">
+        <f t="shared" si="14"/>
+        <v>0.19906348604892404</v>
+      </c>
+      <c r="P61" s="16">
+        <f t="shared" si="15"/>
+        <v>0.72236828272499465</v>
+      </c>
+      <c r="Q61" s="16">
+        <f t="shared" si="16"/>
+        <v>0.76972186621268446</v>
+      </c>
+      <c r="R61" s="16">
+        <f t="shared" si="17"/>
+        <v>1.2739787006823047</v>
+      </c>
+      <c r="S61" s="16">
+        <f t="shared" si="18"/>
+        <v>1.3111327593880611</v>
+      </c>
+      <c r="T61" s="17">
+        <f t="shared" si="19"/>
+        <v>0.33024811931729431</v>
+      </c>
+    </row>
+    <row r="62" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A62" s="11">
+        <v>1000</v>
+      </c>
+      <c r="B62" s="11">
+        <v>5118.34</v>
+      </c>
+      <c r="C62" s="11">
+        <v>4944.0569999999998</v>
+      </c>
+      <c r="D62" s="11">
+        <v>4234.7340000000004</v>
+      </c>
+      <c r="E62" s="11">
+        <v>5362.3980000000001</v>
+      </c>
+      <c r="F62" s="11">
+        <v>3142.93</v>
+      </c>
+      <c r="G62" s="11">
+        <v>1817.213</v>
+      </c>
+      <c r="H62" s="11">
+        <v>1699.385</v>
+      </c>
+      <c r="I62" s="11">
+        <v>1797.4390000000001</v>
+      </c>
+      <c r="J62" s="11">
+        <v>3104.5079999999998</v>
+      </c>
+      <c r="L62" s="15">
+        <f t="shared" si="11"/>
+        <v>0.87984445517567578</v>
+      </c>
+      <c r="M62" s="16">
+        <f t="shared" si="12"/>
+        <v>0.95788409202761882</v>
+      </c>
+      <c r="N62" s="16">
+        <f t="shared" si="13"/>
+        <v>0.83568969857537612</v>
+      </c>
+      <c r="O62" s="16">
+        <f t="shared" si="14"/>
+        <v>0.38525664330362114</v>
+      </c>
+      <c r="P62" s="16">
+        <f t="shared" si="15"/>
+        <v>1.0257481106060407</v>
+      </c>
+      <c r="Q62" s="16">
+        <f t="shared" si="16"/>
+        <v>0.88592289373706912</v>
+      </c>
+      <c r="R62" s="16">
+        <f t="shared" si="17"/>
+        <v>1.6934361810676573</v>
+      </c>
+      <c r="S62" s="16">
+        <f t="shared" si="18"/>
+        <v>1.4208726223070984</v>
+      </c>
+      <c r="T62" s="17">
+        <f t="shared" si="19"/>
+        <v>0.13062602120256203</v>
+      </c>
+    </row>
+    <row r="63" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A63" s="11">
+        <v>2000</v>
+      </c>
+      <c r="B63" s="11">
+        <v>6463.9340000000002</v>
+      </c>
+      <c r="C63" s="11">
+        <v>5969.0569999999998</v>
+      </c>
+      <c r="D63" s="11">
+        <v>4691.393</v>
+      </c>
+      <c r="E63" s="11">
+        <v>6115.3689999999997</v>
+      </c>
+      <c r="F63" s="11">
+        <v>3701.0250000000001</v>
+      </c>
+      <c r="G63" s="11">
+        <v>2066.0859999999998</v>
+      </c>
+      <c r="H63" s="11">
+        <v>1632.787</v>
+      </c>
+      <c r="I63" s="11">
+        <v>1801.9469999999999</v>
+      </c>
+      <c r="J63" s="11">
+        <v>4471.9260000000004</v>
+      </c>
+      <c r="L63" s="15">
+        <f t="shared" si="11"/>
+        <v>0.43539915012091424</v>
+      </c>
+      <c r="M63" s="16">
+        <f t="shared" si="12"/>
+        <v>0.54817919436790075</v>
+      </c>
+      <c r="N63" s="16">
+        <f t="shared" si="13"/>
+        <v>0.13038487124994388</v>
+      </c>
+      <c r="O63" s="16">
+        <f t="shared" si="14"/>
+        <v>0.32919453887356326</v>
+      </c>
+      <c r="P63" s="16">
+        <f t="shared" si="15"/>
+        <v>-0.12047377420705405</v>
+      </c>
+      <c r="Q63" s="16">
+        <f t="shared" si="16"/>
+        <v>-0.10341473177712698</v>
+      </c>
+      <c r="R63" s="16">
+        <f t="shared" si="17"/>
+        <v>1.616228341508634</v>
+      </c>
+      <c r="S63" s="16">
+        <f t="shared" si="18"/>
+        <v>1.6593524691996586</v>
+      </c>
+      <c r="T63" s="17">
+        <f t="shared" si="19"/>
+        <v>0.10140789173811256</v>
+      </c>
+    </row>
+    <row r="64" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A64" s="11">
+        <v>2500</v>
+      </c>
+      <c r="B64" s="11">
+        <v>6794.57</v>
+      </c>
+      <c r="C64" s="11">
+        <v>5927.049</v>
+      </c>
+      <c r="D64" s="11">
+        <v>5077.7659999999996</v>
+      </c>
+      <c r="E64" s="11">
+        <v>6654.8159999999998</v>
+      </c>
+      <c r="F64" s="11">
+        <v>4116.393</v>
+      </c>
+      <c r="G64" s="11">
+        <v>1853.893</v>
+      </c>
+      <c r="H64" s="11">
+        <v>1728.1759999999999</v>
+      </c>
+      <c r="I64" s="11">
+        <v>2014.9590000000001</v>
+      </c>
+      <c r="J64" s="11">
+        <v>4583.7089999999998</v>
+      </c>
+      <c r="L64" s="15">
+        <f t="shared" si="11"/>
+        <v>0.23155453767767495</v>
+      </c>
+      <c r="M64" s="16">
+        <f t="shared" si="12"/>
+        <v>0.69252070688491429</v>
+      </c>
+      <c r="N64" s="16">
+        <f t="shared" si="13"/>
+        <v>0.5576977626910421</v>
+      </c>
+      <c r="O64" s="16">
+        <f t="shared" si="14"/>
+        <v>0.27501871261315575</v>
+      </c>
+      <c r="P64" s="16">
+        <f t="shared" si="15"/>
+        <v>0.43514525311843849</v>
+      </c>
+      <c r="Q64" s="16">
+        <f t="shared" si="16"/>
+        <v>0.18270006779665129</v>
+      </c>
+      <c r="R64" s="16">
+        <f t="shared" si="17"/>
+        <v>1.4259153775526787</v>
+      </c>
+      <c r="S64" s="16">
+        <f t="shared" si="18"/>
+        <v>1.4030949496159248</v>
+      </c>
+      <c r="T64" s="17">
+        <f t="shared" si="19"/>
+        <v>-0.30438580029422119</v>
+      </c>
+    </row>
+    <row r="65" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A65" s="11">
+        <v>3800</v>
+      </c>
+      <c r="B65" s="11">
+        <v>7588.1149999999998</v>
+      </c>
+      <c r="C65" s="11">
+        <v>6774.3850000000002</v>
+      </c>
+      <c r="D65" s="11">
+        <v>5876.6390000000001</v>
+      </c>
+      <c r="E65" s="11">
+        <v>8123.77</v>
+      </c>
+      <c r="F65" s="11">
+        <v>5009.6310000000003</v>
+      </c>
+      <c r="G65" s="11">
+        <v>2255.5329999999999</v>
+      </c>
+      <c r="H65" s="11">
+        <v>1950</v>
+      </c>
+      <c r="I65" s="11">
+        <v>2244.98</v>
+      </c>
+      <c r="J65" s="11">
+        <v>4586.68</v>
+      </c>
+      <c r="L65" s="15">
+        <f t="shared" si="11"/>
+        <v>-0.64561813562625703</v>
+      </c>
+      <c r="M65" s="16">
+        <f t="shared" si="12"/>
+        <v>-0.59392735541912156</v>
+      </c>
+      <c r="N65" s="16">
+        <f t="shared" si="13"/>
+        <v>-0.38016086123193238</v>
+      </c>
+      <c r="O65" s="16">
+        <f t="shared" si="14"/>
+        <v>-0.50299141112416135</v>
+      </c>
+      <c r="P65" s="16">
+        <f t="shared" si="15"/>
+        <v>-0.95998557436106335</v>
+      </c>
+      <c r="Q65" s="16">
+        <f t="shared" si="16"/>
+        <v>-5.9207001256606176E-2</v>
+      </c>
+      <c r="R65" s="16">
+        <f t="shared" si="17"/>
+        <v>0.59945579221105549</v>
+      </c>
+      <c r="S65" s="16">
+        <f t="shared" si="18"/>
+        <v>0.54174573348698185</v>
+      </c>
+      <c r="T65" s="17">
+        <f t="shared" si="19"/>
+        <v>-0.46900339412717756</v>
+      </c>
+    </row>
+    <row r="66" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A66" s="11">
+        <v>5000</v>
+      </c>
+      <c r="B66" s="11">
+        <v>6777.152</v>
+      </c>
+      <c r="C66" s="11">
+        <v>5945.6970000000001</v>
+      </c>
+      <c r="D66" s="11">
+        <v>4919.2619999999997</v>
+      </c>
+      <c r="E66" s="11">
+        <v>6480.84</v>
+      </c>
+      <c r="F66" s="11">
+        <v>4406.9669999999996</v>
+      </c>
+      <c r="G66" s="11">
+        <v>1790.6759999999999</v>
+      </c>
+      <c r="H66" s="11">
+        <v>1740.3689999999999</v>
+      </c>
+      <c r="I66" s="11">
+        <v>1974.693</v>
+      </c>
+      <c r="J66" s="11">
+        <v>3491.4960000000001</v>
+      </c>
+      <c r="L66" s="15">
+        <f t="shared" si="11"/>
+        <v>0.52001863998990561</v>
+      </c>
+      <c r="M66" s="16">
+        <f t="shared" si="12"/>
+        <v>0.45642734136458185</v>
+      </c>
+      <c r="N66" s="16">
+        <f t="shared" si="13"/>
+        <v>0.74729095613225571</v>
+      </c>
+      <c r="O66" s="16">
+        <f t="shared" si="14"/>
+        <v>0.48879959719807997</v>
+      </c>
+      <c r="P66" s="16">
+        <f t="shared" si="15"/>
+        <v>0.69285882082982408</v>
+      </c>
+      <c r="Q66" s="16">
+        <f t="shared" si="16"/>
+        <v>-0.24422864392037869</v>
+      </c>
+      <c r="R66" s="16">
+        <f t="shared" si="17"/>
+        <v>1.1133256008294063</v>
+      </c>
+      <c r="S66" s="16">
+        <f t="shared" si="18"/>
+        <v>1.385328186482464</v>
+      </c>
+      <c r="T66" s="17">
+        <f t="shared" si="19"/>
+        <v>-0.21827164180474595</v>
+      </c>
+    </row>
+    <row r="67" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A67" s="11">
+        <v>10000</v>
+      </c>
+      <c r="B67" s="11">
+        <v>5714.857</v>
+      </c>
+      <c r="C67" s="11">
+        <v>8814.0370000000003</v>
+      </c>
+      <c r="D67" s="11">
+        <v>3658.299</v>
+      </c>
+      <c r="E67" s="11">
+        <v>5161.7830000000004</v>
+      </c>
+      <c r="F67" s="11">
+        <v>3658.402</v>
+      </c>
+      <c r="G67" s="11">
+        <v>1660.6559999999999</v>
+      </c>
+      <c r="H67" s="11">
+        <v>4911.5780000000004</v>
+      </c>
+      <c r="I67" s="11">
+        <v>3018.5450000000001</v>
+      </c>
+      <c r="J67" s="11">
+        <v>1458.5039999999999</v>
+      </c>
+      <c r="L67" s="18">
+        <f t="shared" si="11"/>
+        <v>-2.030646205128908</v>
+      </c>
+      <c r="M67" s="19">
+        <f t="shared" si="12"/>
+        <v>-1.3590186026654751</v>
+      </c>
+      <c r="N67" s="19">
+        <f t="shared" si="13"/>
+        <v>-0.54057673620317737</v>
+      </c>
+      <c r="O67" s="19">
+        <f t="shared" si="14"/>
+        <v>-1.6492955058448162</v>
+      </c>
+      <c r="P67" s="19">
+        <f t="shared" si="15"/>
+        <v>-1.4407446505529755</v>
+      </c>
+      <c r="Q67" s="19">
+        <f t="shared" si="16"/>
+        <v>0.43104790755044647</v>
+      </c>
+      <c r="R67" s="19">
+        <f t="shared" si="17"/>
+        <v>-1.4206801820659967</v>
+      </c>
+      <c r="S67" s="19">
+        <f t="shared" si="18"/>
+        <v>-2.1394107808216183</v>
+      </c>
+      <c r="T67" s="20">
+        <f t="shared" si="19"/>
+        <v>0.24289058950118475</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G29"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I31" sqref="I31"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="25.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="29" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1993</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>3137.424</v>
+      </c>
+      <c r="D3" s="21">
+        <v>3097.2011265871329</v>
+      </c>
+      <c r="E3">
+        <f>(C3-D3)/D3*100</f>
+        <v>1.2986845790408672</v>
+      </c>
+      <c r="F3" s="21">
+        <v>3138.2244207466119</v>
+      </c>
+      <c r="G3">
+        <f>(C3-F3)/F3*100</f>
+        <v>-2.5505529219657756E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>1993</v>
+      </c>
+      <c r="B4">
+        <v>2</v>
+      </c>
+      <c r="C4">
+        <v>2897.5529999999999</v>
+      </c>
+      <c r="D4" s="22">
+        <v>2828.043843703063</v>
+      </c>
+      <c r="E4">
+        <f t="shared" ref="E4:E29" si="0">(C4-D4)/D4*100</f>
+        <v>2.4578528530138017</v>
+      </c>
+      <c r="F4" s="22">
+        <v>2869.9033992098362</v>
+      </c>
+      <c r="G4">
+        <f t="shared" ref="G4:G29" si="1">(C4-F4)/F4*100</f>
+        <v>0.96343315241120775</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>1993</v>
+      </c>
+      <c r="B5">
+        <v>3</v>
+      </c>
+      <c r="C5">
+        <v>3213.5610000000001</v>
+      </c>
+      <c r="D5" s="22">
+        <v>3124.6219133297382</v>
+      </c>
+      <c r="E5">
+        <f t="shared" si="0"/>
+        <v>2.8463951523493116</v>
+      </c>
+      <c r="F5" s="22">
+        <v>3163.7328086568314</v>
+      </c>
+      <c r="G5">
+        <f t="shared" si="1"/>
+        <v>1.5749810226333063</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>1993</v>
+      </c>
+      <c r="B6">
+        <v>4</v>
+      </c>
+      <c r="C6">
+        <v>3719.9850000000001</v>
+      </c>
+      <c r="D6" s="22">
+        <v>3767.9021887185909</v>
+      </c>
+      <c r="E6">
+        <f t="shared" si="0"/>
+        <v>-1.2717206105312062</v>
+      </c>
+      <c r="F6" s="22">
+        <v>3744.5980348770508</v>
+      </c>
+      <c r="G6">
+        <f t="shared" si="1"/>
+        <v>-0.65729444516623159</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>1993</v>
+      </c>
+      <c r="B7">
+        <v>5</v>
+      </c>
+      <c r="C7">
+        <v>3304.7469999999998</v>
+      </c>
+      <c r="D7" s="22">
+        <v>3287.1189562489189</v>
+      </c>
+      <c r="E7">
+        <f t="shared" si="0"/>
+        <v>0.5362764166952162</v>
+      </c>
+      <c r="F7" s="22">
+        <v>3347.4428289025609</v>
+      </c>
+      <c r="G7">
+        <f t="shared" si="1"/>
+        <v>-1.2754759703113028</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>1993</v>
+      </c>
+      <c r="B8">
+        <v>6</v>
+      </c>
+      <c r="C8">
+        <v>3104.9870000000001</v>
+      </c>
+      <c r="D8" s="22">
+        <v>3091.1334493877594</v>
+      </c>
+      <c r="E8">
+        <f t="shared" si="0"/>
+        <v>0.44817057687964285</v>
+      </c>
+      <c r="F8" s="22">
+        <v>3149.6888761198761</v>
+      </c>
+      <c r="G8">
+        <f t="shared" si="1"/>
+        <v>-1.4192473567403452</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>1993</v>
+      </c>
+      <c r="B9">
+        <v>7</v>
+      </c>
+      <c r="C9">
+        <v>3034.0120000000002</v>
+      </c>
+      <c r="D9" s="22">
+        <v>3135.5221601011058</v>
+      </c>
+      <c r="E9">
+        <f t="shared" si="0"/>
+        <v>-3.2374244198558748</v>
+      </c>
+      <c r="F9" s="22">
+        <v>3078.4479236557354</v>
+      </c>
+      <c r="G9">
+        <f t="shared" si="1"/>
+        <v>-1.4434521797258935</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>1993</v>
+      </c>
+      <c r="B10">
+        <v>8</v>
+      </c>
+      <c r="C10">
+        <v>2943.6990000000001</v>
+      </c>
+      <c r="D10" s="22">
+        <v>2252.4940797195004</v>
+      </c>
+      <c r="E10">
+        <f t="shared" si="0"/>
+        <v>30.686203639948051</v>
+      </c>
+      <c r="F10" s="22">
+        <v>2987.7651938831946</v>
+      </c>
+      <c r="G10">
+        <f t="shared" si="1"/>
+        <v>-1.4748881195018448</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>1993</v>
+      </c>
+      <c r="B11">
+        <v>9</v>
+      </c>
+      <c r="C11">
+        <v>2966.241</v>
+      </c>
+      <c r="D11" s="22">
+        <v>2586.6243169208715</v>
+      </c>
+      <c r="E11">
+        <f t="shared" si="0"/>
+        <v>14.67614297893193</v>
+      </c>
+      <c r="F11" s="22">
+        <v>3010.3990374026703</v>
+      </c>
+      <c r="G11">
+        <f t="shared" si="1"/>
+        <v>-1.4668499708520111</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>1993</v>
+      </c>
+      <c r="B12">
+        <v>10</v>
+      </c>
+      <c r="C12">
+        <v>3034.0120000000002</v>
+      </c>
+      <c r="D12" s="22">
+        <v>2738.0414190908305</v>
+      </c>
+      <c r="E12">
+        <f t="shared" si="0"/>
+        <v>10.809572815280751</v>
+      </c>
+      <c r="F12" s="22">
+        <v>3078.4479236557354</v>
+      </c>
+      <c r="G12">
+        <f t="shared" si="1"/>
+        <v>-1.4434521797258935</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>1993</v>
+      </c>
+      <c r="B13">
+        <v>11</v>
+      </c>
+      <c r="C13">
+        <v>3034.0120000000002</v>
+      </c>
+      <c r="D13" s="22">
+        <v>3135.5221601011058</v>
+      </c>
+      <c r="E13">
+        <f t="shared" si="0"/>
+        <v>-3.2374244198558748</v>
+      </c>
+      <c r="F13" s="22">
+        <v>3078.4479236557354</v>
+      </c>
+      <c r="G13">
+        <f t="shared" si="1"/>
+        <v>-1.4434521797258935</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>1993</v>
+      </c>
+      <c r="B14">
+        <v>12</v>
+      </c>
+      <c r="C14">
+        <v>3217.5830000000001</v>
+      </c>
+      <c r="D14" s="23">
+        <v>3091.1334493877594</v>
+      </c>
+      <c r="E14">
+        <f t="shared" si="0"/>
+        <v>4.090717941578542</v>
+      </c>
+      <c r="F14" s="23">
+        <v>3262.7085831230524</v>
+      </c>
+      <c r="G14">
+        <f t="shared" si="1"/>
+        <v>-1.3830712113387191</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>15</v>
+      </c>
+      <c r="B17" t="s">
+        <v>16</v>
+      </c>
+      <c r="C17" t="s">
+        <v>17</v>
+      </c>
+      <c r="D17" t="s">
+        <v>18</v>
+      </c>
+      <c r="E17" t="s">
+        <v>14</v>
+      </c>
+      <c r="F17" t="s">
+        <v>22</v>
+      </c>
+      <c r="G17" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>1993</v>
+      </c>
+      <c r="B18">
+        <v>1</v>
+      </c>
+      <c r="C18">
+        <v>5118.03</v>
+      </c>
+      <c r="D18" s="21">
+        <v>4954.3282301907293</v>
+      </c>
+      <c r="E18">
+        <f t="shared" si="0"/>
+        <v>3.3042172864466903</v>
+      </c>
+      <c r="F18" s="21">
+        <v>4953.5307084685246</v>
+      </c>
+      <c r="G18">
+        <f t="shared" si="1"/>
+        <v>3.3208493337943414</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>1993</v>
+      </c>
+      <c r="B19">
+        <v>2</v>
+      </c>
+      <c r="C19">
+        <v>4234.973</v>
+      </c>
+      <c r="D19" s="22">
+        <v>4135.0791901829816</v>
+      </c>
+      <c r="E19">
+        <f t="shared" si="0"/>
+        <v>2.4157653390090923</v>
+      </c>
+      <c r="F19" s="22">
+        <v>4137.8086222950851</v>
+      </c>
+      <c r="G19">
+        <f t="shared" si="1"/>
+        <v>2.3482085947953162</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>1993</v>
+      </c>
+      <c r="B20">
+        <v>3</v>
+      </c>
+      <c r="C20">
+        <v>4501.1289999999999</v>
+      </c>
+      <c r="D20" s="22">
+        <v>4338.1466084448675</v>
+      </c>
+      <c r="E20">
+        <f t="shared" si="0"/>
+        <v>3.7569590487758568</v>
+      </c>
+      <c r="F20" s="22">
+        <v>4340.9253478426263</v>
+      </c>
+      <c r="G20">
+        <f t="shared" si="1"/>
+        <v>3.6905415163841147</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>1993</v>
+      </c>
+      <c r="B21">
+        <v>4</v>
+      </c>
+      <c r="C21">
+        <v>6541.527</v>
+      </c>
+      <c r="D21" s="22">
+        <v>6560.9276966643783</v>
+      </c>
+      <c r="E21">
+        <f t="shared" si="0"/>
+        <v>-0.29570051007027176</v>
+      </c>
+      <c r="F21" s="22">
+        <v>6574.9887241879096</v>
+      </c>
+      <c r="G21">
+        <f t="shared" si="1"/>
+        <v>-0.50892443457448655</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>1993</v>
+      </c>
+      <c r="B22">
+        <v>5</v>
+      </c>
+      <c r="C22">
+        <v>8354.8520000000008</v>
+      </c>
+      <c r="D22" s="22">
+        <v>8340.569569466712</v>
+      </c>
+      <c r="E22">
+        <f t="shared" si="0"/>
+        <v>0.17124047002226483</v>
+      </c>
+      <c r="F22" s="22">
+        <v>8379.725597745186</v>
+      </c>
+      <c r="G22">
+        <f t="shared" si="1"/>
+        <v>-0.29683069517071248</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>1993</v>
+      </c>
+      <c r="B23">
+        <v>6</v>
+      </c>
+      <c r="C23">
+        <v>8227.0759999999991</v>
+      </c>
+      <c r="D23" s="22">
+        <v>8206.937686151181</v>
+      </c>
+      <c r="E23">
+        <f t="shared" si="0"/>
+        <v>0.24538158590871958</v>
+      </c>
+      <c r="F23" s="22">
+        <v>8246.1018641805367</v>
+      </c>
+      <c r="G23">
+        <f t="shared" si="1"/>
+        <v>-0.2307255536483519</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>1993</v>
+      </c>
+      <c r="B24">
+        <v>7</v>
+      </c>
+      <c r="C24">
+        <v>8181.6769999999997</v>
+      </c>
+      <c r="D24" s="22">
+        <v>8236.6266059642694</v>
+      </c>
+      <c r="E24">
+        <f t="shared" si="0"/>
+        <v>-0.66713727103374898</v>
+      </c>
+      <c r="F24" s="22">
+        <v>8198.4531063967261</v>
+      </c>
+      <c r="G24">
+        <f t="shared" si="1"/>
+        <v>-0.20462526502270378</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>1993</v>
+      </c>
+      <c r="B25">
+        <v>8</v>
+      </c>
+      <c r="C25">
+        <v>7927.7449999999999</v>
+      </c>
+      <c r="D25" s="22">
+        <v>7219.8616266660447</v>
+      </c>
+      <c r="E25">
+        <f t="shared" si="0"/>
+        <v>9.8046667642415528</v>
+      </c>
+      <c r="F25" s="22">
+        <v>7950.4075580702847</v>
+      </c>
+      <c r="G25">
+        <f t="shared" si="1"/>
+        <v>-0.28504901044073599</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>1993</v>
+      </c>
+      <c r="B26">
+        <v>9</v>
+      </c>
+      <c r="C26">
+        <v>7961.3119999999999</v>
+      </c>
+      <c r="D26" s="22">
+        <v>7603.9543412227085</v>
+      </c>
+      <c r="E26">
+        <f t="shared" si="0"/>
+        <v>4.6996292026633686</v>
+      </c>
+      <c r="F26" s="22">
+        <v>7985.4244644118426</v>
+      </c>
+      <c r="G26">
+        <f t="shared" si="1"/>
+        <v>-0.3019559513624257</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>1993</v>
+      </c>
+      <c r="B27">
+        <v>10</v>
+      </c>
+      <c r="C27">
+        <v>7896.8770000000004</v>
+      </c>
+      <c r="D27" s="22">
+        <v>7363.7031881184812</v>
+      </c>
+      <c r="E27">
+        <f t="shared" si="0"/>
+        <v>7.24056630557582</v>
+      </c>
+      <c r="F27" s="22">
+        <v>7944.0689292140032</v>
+      </c>
+      <c r="G27">
+        <f t="shared" si="1"/>
+        <v>-0.594052363272634</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>1993</v>
+      </c>
+      <c r="B28">
+        <v>11</v>
+      </c>
+      <c r="C28">
+        <v>5350.1009999999997</v>
+      </c>
+      <c r="D28" s="22">
+        <v>5182.2011812916144</v>
+      </c>
+      <c r="E28">
+        <f t="shared" si="0"/>
+        <v>3.2399324695174774</v>
+      </c>
+      <c r="F28" s="22">
+        <v>5186.9389289586888</v>
+      </c>
+      <c r="G28">
+        <f t="shared" si="1"/>
+        <v>3.145633161986479</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>1993</v>
+      </c>
+      <c r="B29">
+        <v>12</v>
+      </c>
+      <c r="C29">
+        <v>8192.8089999999993</v>
+      </c>
+      <c r="D29" s="23">
+        <v>8206.937686151181</v>
+      </c>
+      <c r="E29">
+        <f t="shared" si="0"/>
+        <v>-0.1721553969518152</v>
+      </c>
+      <c r="F29" s="23">
+        <v>8269.6009209654567</v>
+      </c>
+      <c r="G29">
+        <f t="shared" si="1"/>
+        <v>-0.9286049193833662</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
revised Cherry Creek info
Made some small revisions after receiving the updated Cherry Creek DSS.
</commit_message>
<xml_diff>
--- a/Cherry_Braid_AQ.xlsx
+++ b/Cherry_Braid_AQ.xlsx
@@ -9,11 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Cherry_Braid_AQ" sheetId="2" r:id="rId1"/>
     <sheet name="10day" sheetId="3" r:id="rId2"/>
+    <sheet name="revisedMon" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="25">
   <si>
     <t>discharge</t>
   </si>
@@ -94,6 +95,12 @@
   </si>
   <si>
     <t>EP edits</t>
+  </si>
+  <si>
+    <t>LFD</t>
+  </si>
+  <si>
+    <t>Min of Baseline 10-day running mean</t>
   </si>
 </sst>
 </file>
@@ -302,7 +309,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -329,6 +336,14 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -609,10 +624,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T67"/>
+  <dimension ref="A1:T68"/>
   <sheetViews>
-    <sheetView topLeftCell="F40" workbookViewId="0">
-      <selection activeCell="O71" sqref="O71"/>
+    <sheetView topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="R58" sqref="R58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -629,6 +644,7 @@
     <col min="12" max="12" width="12.7109375" bestFit="1" customWidth="1"/>
     <col min="14" max="16" width="12.7109375" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="12.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.25">
@@ -4209,6 +4225,44 @@
         <v>0.24289058950118475</v>
       </c>
     </row>
+    <row r="68" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="L68" s="24">
+        <f>MAX(L48:L67)</f>
+        <v>0.87984445517567578</v>
+      </c>
+      <c r="M68" s="24">
+        <f t="shared" ref="M68:T68" si="20">MAX(M48:M67)</f>
+        <v>1.0688126303196868</v>
+      </c>
+      <c r="N68" s="24">
+        <f t="shared" si="20"/>
+        <v>0.83568969857537612</v>
+      </c>
+      <c r="O68" s="24">
+        <f t="shared" si="20"/>
+        <v>0.48879959719807997</v>
+      </c>
+      <c r="P68" s="24">
+        <f t="shared" si="20"/>
+        <v>1.0257481106060407</v>
+      </c>
+      <c r="Q68" s="24">
+        <f t="shared" si="20"/>
+        <v>1.2859365823844398</v>
+      </c>
+      <c r="R68" s="24">
+        <f t="shared" si="20"/>
+        <v>3.0015501518644232</v>
+      </c>
+      <c r="S68" s="24">
+        <f t="shared" si="20"/>
+        <v>1.6593524691996586</v>
+      </c>
+      <c r="T68" s="24">
+        <f t="shared" si="20"/>
+        <v>0.33892918926757221</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
@@ -4219,8 +4273,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I31" sqref="I31"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4889,4 +4943,479 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E26"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="16.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="25" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" s="25"/>
+      <c r="C1" s="25"/>
+      <c r="D1" s="25"/>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="25" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" s="25" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" s="25" t="s">
+        <v>17</v>
+      </c>
+      <c r="D2" s="25" t="s">
+        <v>24</v>
+      </c>
+      <c r="E2" s="25" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="29">
+        <v>1984</v>
+      </c>
+      <c r="B3" s="29">
+        <v>1</v>
+      </c>
+      <c r="C3" s="29">
+        <v>7748.4049999999997</v>
+      </c>
+      <c r="D3" s="26">
+        <v>6718.8953122735566</v>
+      </c>
+      <c r="E3">
+        <f>(C3-D3)/D3*100</f>
+        <v>15.322603491764708</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="29">
+        <v>1984</v>
+      </c>
+      <c r="B4" s="29">
+        <v>2</v>
+      </c>
+      <c r="C4" s="29">
+        <v>8057.4080000000004</v>
+      </c>
+      <c r="D4" s="27">
+        <v>8112.5945476510042</v>
+      </c>
+      <c r="E4">
+        <f t="shared" ref="E4:E26" si="0">(C4-D4)/D4*100</f>
+        <v>-0.68025768238328932</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="29">
+        <v>1984</v>
+      </c>
+      <c r="B5" s="29">
+        <v>3</v>
+      </c>
+      <c r="C5" s="29">
+        <v>7864.0079999999998</v>
+      </c>
+      <c r="D5" s="27">
+        <v>7919.6675096679301</v>
+      </c>
+      <c r="E5">
+        <f t="shared" si="0"/>
+        <v>-0.70280109108095679</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="29">
+        <v>1984</v>
+      </c>
+      <c r="B6" s="29">
+        <v>4</v>
+      </c>
+      <c r="C6" s="29">
+        <v>7590.4380000000001</v>
+      </c>
+      <c r="D6" s="27">
+        <v>7646.7660521312591</v>
+      </c>
+      <c r="E6">
+        <f t="shared" si="0"/>
+        <v>-0.7366258068737388</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="29">
+        <v>1984</v>
+      </c>
+      <c r="B7" s="29">
+        <v>5</v>
+      </c>
+      <c r="C7" s="29">
+        <v>7029.9340000000002</v>
+      </c>
+      <c r="D7" s="27">
+        <v>7091.9411837111284</v>
+      </c>
+      <c r="E7">
+        <f t="shared" si="0"/>
+        <v>-0.87433302257987067</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="29">
+        <v>1984</v>
+      </c>
+      <c r="B8" s="29">
+        <v>6</v>
+      </c>
+      <c r="C8" s="29">
+        <v>6424.018</v>
+      </c>
+      <c r="D8" s="27">
+        <v>6867.779557361835</v>
+      </c>
+      <c r="E8">
+        <f t="shared" si="0"/>
+        <v>-6.4614997271738295</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="29">
+        <v>1984</v>
+      </c>
+      <c r="B9" s="29">
+        <v>7</v>
+      </c>
+      <c r="C9" s="29">
+        <v>6273.5990000000002</v>
+      </c>
+      <c r="D9" s="27">
+        <v>6812.0448674684767</v>
+      </c>
+      <c r="E9">
+        <f t="shared" si="0"/>
+        <v>-7.9043206253657035</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="29">
+        <v>1984</v>
+      </c>
+      <c r="B10" s="29">
+        <v>8</v>
+      </c>
+      <c r="C10" s="29">
+        <v>7179.8609999999999</v>
+      </c>
+      <c r="D10" s="27">
+        <v>7236.7399373190592</v>
+      </c>
+      <c r="E10">
+        <f t="shared" si="0"/>
+        <v>-0.78597459369433753</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="29">
+        <v>1984</v>
+      </c>
+      <c r="B11" s="29">
+        <v>9</v>
+      </c>
+      <c r="C11" s="29">
+        <v>6752.7250000000004</v>
+      </c>
+      <c r="D11" s="27">
+        <v>6619.5646872032867</v>
+      </c>
+      <c r="E11">
+        <f t="shared" si="0"/>
+        <v>2.0116173659294336</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="29">
+        <v>1984</v>
+      </c>
+      <c r="B12" s="29">
+        <v>10</v>
+      </c>
+      <c r="C12" s="29">
+        <v>7003.0860000000002</v>
+      </c>
+      <c r="D12" s="27">
+        <v>6946.6071514361884</v>
+      </c>
+      <c r="E12">
+        <f t="shared" si="0"/>
+        <v>0.81304221373933694</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="29">
+        <v>1984</v>
+      </c>
+      <c r="B13" s="29">
+        <v>11</v>
+      </c>
+      <c r="C13" s="29">
+        <v>7361.2439999999997</v>
+      </c>
+      <c r="D13" s="27">
+        <v>7331.1336454300108</v>
+      </c>
+      <c r="E13">
+        <f t="shared" si="0"/>
+        <v>0.41071894233927514</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="29">
+        <v>1984</v>
+      </c>
+      <c r="B14" s="29">
+        <v>12</v>
+      </c>
+      <c r="C14" s="29">
+        <v>4886.4709999999995</v>
+      </c>
+      <c r="D14" s="28">
+        <v>4594.8969082824842</v>
+      </c>
+      <c r="E14">
+        <f t="shared" si="0"/>
+        <v>6.3456068229069826</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="29">
+        <v>1985</v>
+      </c>
+      <c r="B15" s="29">
+        <v>1</v>
+      </c>
+      <c r="C15" s="29">
+        <v>5357.7160000000003</v>
+      </c>
+      <c r="D15" s="26">
+        <v>5264.4312114547547</v>
+      </c>
+      <c r="E15">
+        <f t="shared" si="0"/>
+        <v>1.7719822863725414</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="29">
+        <v>1985</v>
+      </c>
+      <c r="B16" s="29">
+        <v>2</v>
+      </c>
+      <c r="C16" s="29">
+        <v>5542.0540000000001</v>
+      </c>
+      <c r="D16" s="27">
+        <v>5182.5759038581982</v>
+      </c>
+      <c r="E16">
+        <f t="shared" si="0"/>
+        <v>6.9362823200367671</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="29">
+        <v>1985</v>
+      </c>
+      <c r="B17" s="29">
+        <v>3</v>
+      </c>
+      <c r="C17" s="29">
+        <v>4949.0940000000001</v>
+      </c>
+      <c r="D17" s="27">
+        <v>4791.0947362276584</v>
+      </c>
+      <c r="E17">
+        <f t="shared" si="0"/>
+        <v>3.2977695593793417</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="29">
+        <v>1985</v>
+      </c>
+      <c r="B18" s="29">
+        <v>4</v>
+      </c>
+      <c r="C18" s="29">
+        <v>7061.0230000000001</v>
+      </c>
+      <c r="D18" s="27">
+        <v>7136.1722140109441</v>
+      </c>
+      <c r="E18">
+        <f t="shared" si="0"/>
+        <v>-1.0530745581419447</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="29">
+        <v>1985</v>
+      </c>
+      <c r="B19" s="29">
+        <v>5</v>
+      </c>
+      <c r="C19" s="29">
+        <v>8172.0969999999998</v>
+      </c>
+      <c r="D19" s="27">
+        <v>8227.4905297205041</v>
+      </c>
+      <c r="E19">
+        <f t="shared" si="0"/>
+        <v>-0.67327369773813817</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="29">
+        <v>1985</v>
+      </c>
+      <c r="B20" s="29">
+        <v>6</v>
+      </c>
+      <c r="C20" s="29">
+        <v>7270.2309999999998</v>
+      </c>
+      <c r="D20" s="27">
+        <v>7327.3420437000805</v>
+      </c>
+      <c r="E20">
+        <f t="shared" si="0"/>
+        <v>-0.77942374410081983</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="29">
+        <v>1985</v>
+      </c>
+      <c r="B21" s="29">
+        <v>7</v>
+      </c>
+      <c r="C21" s="29">
+        <v>7159.7039999999997</v>
+      </c>
+      <c r="D21" s="27">
+        <v>7217.0846895761697</v>
+      </c>
+      <c r="E21">
+        <f t="shared" si="0"/>
+        <v>-0.79506742742047143</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="29">
+        <v>1985</v>
+      </c>
+      <c r="B22" s="29">
+        <v>8</v>
+      </c>
+      <c r="C22" s="29">
+        <v>7508.2259999999997</v>
+      </c>
+      <c r="D22" s="27">
+        <v>7564.7551876387397</v>
+      </c>
+      <c r="E22">
+        <f t="shared" si="0"/>
+        <v>-0.74727054923220904</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="29">
+        <v>1985</v>
+      </c>
+      <c r="B23" s="29">
+        <v>9</v>
+      </c>
+      <c r="C23" s="29">
+        <v>7538.5630000000001</v>
+      </c>
+      <c r="D23" s="27">
+        <v>7595.0174035929904</v>
+      </c>
+      <c r="E23">
+        <f t="shared" si="0"/>
+        <v>-0.74330841646634382</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="29">
+        <v>1985</v>
+      </c>
+      <c r="B24" s="29">
+        <v>10</v>
+      </c>
+      <c r="C24" s="29">
+        <v>7420.8469999999998</v>
+      </c>
+      <c r="D24" s="27">
+        <v>7384.1181774729284</v>
+      </c>
+      <c r="E24">
+        <f t="shared" si="0"/>
+        <v>0.49740296192877353</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" s="29">
+        <v>1985</v>
+      </c>
+      <c r="B25" s="29">
+        <v>11</v>
+      </c>
+      <c r="C25" s="29">
+        <v>5945.7330000000002</v>
+      </c>
+      <c r="D25" s="27">
+        <v>5934.267547380985</v>
+      </c>
+      <c r="E25">
+        <f t="shared" si="0"/>
+        <v>0.19320754461222986</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" s="29">
+        <v>1985</v>
+      </c>
+      <c r="B26" s="29">
+        <v>12</v>
+      </c>
+      <c r="C26" s="29">
+        <v>6199.9809999999998</v>
+      </c>
+      <c r="D26" s="28">
+        <v>6212.5463378567647</v>
+      </c>
+      <c r="E26">
+        <f t="shared" si="0"/>
+        <v>-0.20225745086514366</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>